<commit_message>
added delete sub processing folders
</commit_message>
<xml_diff>
--- a/experiments/kinetics summary.xlsx
+++ b/experiments/kinetics summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CyCIF PC\Documents\GitHub\AutoCIF\experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike\Documents\GitHub\AutoCIF\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56A30F9-78BB-40DB-9339-D57A26A31D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35EF9F4-7999-4A39-8A86-8290ACD53B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{820A76F4-3CAC-4EB4-8A66-C84A0AEDA527}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{820A76F4-3CAC-4EB4-8A66-C84A0AEDA527}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>Stain</t>
   </si>
@@ -514,21 +514,21 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" customWidth="1"/>
-    <col min="5" max="5" width="25.81640625" customWidth="1"/>
-    <col min="6" max="6" width="21.81640625" customWidth="1"/>
-    <col min="7" max="7" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -561,11 +561,20 @@
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>91</v>
+      </c>
+      <c r="E2">
+        <v>63</v>
+      </c>
+      <c r="F2">
+        <v>18.8</v>
+      </c>
+      <c r="G2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -575,11 +584,20 @@
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <v>89</v>
+      </c>
+      <c r="E3">
+        <v>61.7</v>
+      </c>
+      <c r="F3">
+        <v>22.5</v>
+      </c>
+      <c r="G3">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -589,8 +607,20 @@
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>134.69999999999999</v>
+      </c>
+      <c r="E4">
+        <v>93.4</v>
+      </c>
+      <c r="F4">
+        <v>7.2</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -600,8 +630,20 @@
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>57.8</v>
+      </c>
+      <c r="G5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -624,7 +666,7 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -647,7 +689,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -658,7 +700,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -669,7 +711,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -680,7 +722,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -703,7 +745,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -726,7 +768,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -737,7 +779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -760,21 +802,21 @@
         <v>119.6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="5" t="s">
         <v>17</v>

</xml_diff>